<commit_message>
Update Webravo Excalibur Scrum Burndown uge3.xlsx
</commit_message>
<xml_diff>
--- a/gruppearbejde/Webravo Excalibur Scrum Burndown uge3.xlsx
+++ b/gruppearbejde/Webravo Excalibur Scrum Burndown uge3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/Excalibur/gruppearbejde/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CACACCC-464B-4040-8562-FB4A98CC5DE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE792D0C-47AB-9149-8723-19836137B04B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1325,16 +1325,16 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>59.5</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>119</c:v>
+                  <c:v>136</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>178.5</c:v>
+                  <c:v>204</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>238</c:v>
+                  <c:v>272</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>#N/A</c:v>
@@ -1524,7 +1524,7 @@
                   <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>#N/A</c:v>
+                  <c:v>204</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>#N/A</c:v>
@@ -1809,12 +1809,15 @@
             <c:strRef>
               <c:f>'Sprint 1 Example'!$C$16:$L$16</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1830,6 +1833,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1870,12 +1876,15 @@
             <c:strRef>
               <c:f>'Sprint 1 Example'!$C$16:$L$16</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1925,12 +1934,15 @@
             <c:strRef>
               <c:f>'Sprint 1 Example'!$C$16:$L$16</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4101,8 +4113,8 @@
   </sheetPr>
   <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="162" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="162" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="12.75" customHeight="1"/>
@@ -4272,7 +4284,7 @@
       <c r="N7" s="17"/>
       <c r="O7" s="122">
         <f>MAX(C16:L16)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P7" s="83"/>
       <c r="Q7" s="81"/>
@@ -4339,19 +4351,19 @@
       </c>
       <c r="C10" s="77">
         <f>IF(LEN(C9)&gt;0,(LOOKUP(9.99999999999999E+307,$C14:$L14))/(COUNT($C$14:$L$14))*C9,"")</f>
-        <v>59.5</v>
+        <v>68</v>
       </c>
       <c r="D10" s="77">
         <f t="shared" ref="D10:H10" si="0">IF(LEN(D9)&gt;0,(LOOKUP(9.99999999999999E+307,$C14:$L14))/(COUNT($C$14:$L$14))*D9,NA())</f>
-        <v>119</v>
+        <v>136</v>
       </c>
       <c r="E10" s="77">
         <f t="shared" si="0"/>
-        <v>178.5</v>
+        <v>204</v>
       </c>
       <c r="F10" s="77">
         <f t="shared" si="0"/>
-        <v>238</v>
+        <v>272</v>
       </c>
       <c r="G10" s="77" t="e">
         <f t="shared" si="0"/>
@@ -4451,11 +4463,11 @@
       </c>
       <c r="E12" s="77">
         <f t="shared" ref="E12" si="5">IF(E9&gt;0,IF(E13=0,D12,$C5-E14),NA())</f>
-        <v>265</v>
+        <v>180</v>
       </c>
       <c r="F12" s="77">
         <f t="shared" ref="F12" si="6">IF(F9&gt;0,IF(F13=0,E12,$C5-F14),NA())</f>
-        <v>265</v>
+        <v>180</v>
       </c>
       <c r="G12" s="77" t="e">
         <f t="shared" ref="G12" si="7">IF(G9&gt;0,IF(G13=0,F12,$C5-G14),NA())</f>
@@ -4485,7 +4497,7 @@
       <c r="N12" s="17"/>
       <c r="O12" s="120">
         <f>LOOKUP(9.99999999999999E+307,$C14:$L14)</f>
-        <v>119</v>
+        <v>204</v>
       </c>
       <c r="P12" s="92" t="s">
         <v>58</v>
@@ -4503,7 +4515,9 @@
       <c r="D13" s="89">
         <v>42</v>
       </c>
-      <c r="E13" s="89"/>
+      <c r="E13" s="89">
+        <v>85</v>
+      </c>
       <c r="F13" s="89"/>
       <c r="G13" s="89"/>
       <c r="H13" s="89"/>
@@ -4533,9 +4547,9 @@
         <f t="shared" ref="D14:F14" si="10">IF(LEN(D13)&gt;0,IF(LEN(D9)&gt;0,C14+D13,NA()),NA())</f>
         <v>119</v>
       </c>
-      <c r="E14" s="87" t="e">
+      <c r="E14" s="87">
         <f t="shared" si="10"/>
-        <v>#N/A</v>
+        <v>204</v>
       </c>
       <c r="F14" s="87" t="e">
         <f t="shared" si="10"/>
@@ -4605,9 +4619,9 @@
         <f>IF(SUM(D17:D24)&gt;0,D9,"")</f>
         <v>2</v>
       </c>
-      <c r="E16" s="70" t="str">
+      <c r="E16" s="70">
         <f t="shared" ref="E16:F16" si="12">IF(SUM(E17:E24)&gt;0,E9,"")</f>
-        <v/>
+        <v>3</v>
       </c>
       <c r="F16" s="70" t="str">
         <f t="shared" si="12"/>
@@ -4657,7 +4671,9 @@
         <f>5+7</f>
         <v>12</v>
       </c>
-      <c r="E17" s="78"/>
+      <c r="E17" s="78">
+        <v>22</v>
+      </c>
       <c r="F17" s="78"/>
       <c r="G17" s="78"/>
       <c r="H17" s="78"/>
@@ -4692,7 +4708,7 @@
       <c r="N18" s="16"/>
       <c r="O18" s="112">
         <f>LOOKUP(9.99999999999999E+307,$C17:$L17)</f>
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="P18" s="90" t="s">
         <v>58</v>
@@ -4761,7 +4777,9 @@
       <c r="D21" s="78">
         <v>5</v>
       </c>
-      <c r="E21" s="78"/>
+      <c r="E21" s="78">
+        <v>5</v>
+      </c>
       <c r="F21" s="78"/>
       <c r="G21" s="78"/>
       <c r="H21" s="78"/>
@@ -4817,7 +4835,7 @@
       <c r="N23" s="17"/>
       <c r="O23" s="100">
         <f>(COUNTIFS(C16:L16,"&gt;0"))/O18</f>
-        <v>0.16666666666666666</v>
+        <v>0.13636363636363635</v>
       </c>
       <c r="P23" s="101"/>
       <c r="Q23" s="19"/>
@@ -4833,7 +4851,9 @@
       <c r="D24" s="78">
         <v>20</v>
       </c>
-      <c r="E24" s="78"/>
+      <c r="E24" s="78">
+        <v>10</v>
+      </c>
       <c r="F24" s="78"/>
       <c r="G24" s="78"/>
       <c r="H24" s="78"/>
@@ -4860,9 +4880,9 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="E25" s="75" t="str">
+      <c r="E25" s="75">
         <f t="shared" si="14"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="F25" s="75" t="str">
         <f t="shared" si="14"/>

</xml_diff>